<commit_message>
added locations2.csv with more info
</commit_message>
<xml_diff>
--- a/location.xlsx
+++ b/location.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16700" tabRatio="500"/>
+    <workbookView xWindow="660" yWindow="0" windowWidth="25600" windowHeight="16720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>id</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>well_id</t>
+  </si>
+  <si>
+    <t>url</t>
   </si>
 </sst>
 </file>
@@ -79,17 +82,230 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="109">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -419,15 +635,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -437,11 +656,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>2950650</v>
       </c>
@@ -451,11 +673,16 @@
       <c r="C2">
         <v>-118.961429</v>
       </c>
-      <c r="D2">
-        <v>2950650</v>
+      <c r="D2" s="1" t="str">
+        <f>CONCATENATE("0", A2)</f>
+        <v>02950650</v>
+      </c>
+      <c r="E2" t="str">
+        <f>CONCATENATE("http://owr.conservation.ca.gov/Well/WellDetailPage.aspx?domsapp=1&amp;apinum=", D2)</f>
+        <v>http://owr.conservation.ca.gov/Well/WellDetailPage.aspx?domsapp=1&amp;apinum=02950650</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2942966</v>
       </c>
@@ -465,11 +692,16 @@
       <c r="C3">
         <v>-118.969678</v>
       </c>
-      <c r="D3">
-        <v>2942966</v>
+      <c r="D3" s="1" t="str">
+        <f t="shared" ref="D3:D9" si="0">CONCATENATE("0", A3)</f>
+        <v>02942966</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E9" si="1">CONCATENATE("http://owr.conservation.ca.gov/Well/WellDetailPage.aspx?domsapp=1&amp;apinum=", D3)</f>
+        <v>http://owr.conservation.ca.gov/Well/WellDetailPage.aspx?domsapp=1&amp;apinum=02942966</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>2958273</v>
       </c>
@@ -479,11 +711,16 @@
       <c r="C4">
         <v>-118.96438999999999</v>
       </c>
-      <c r="D4">
-        <v>2958273</v>
+      <c r="D4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>02958273</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>http://owr.conservation.ca.gov/Well/WellDetailPage.aspx?domsapp=1&amp;apinum=02958273</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>2912624</v>
       </c>
@@ -493,11 +730,16 @@
       <c r="C5">
         <v>-118.93161499999999</v>
       </c>
-      <c r="D5">
-        <v>2912624</v>
+      <c r="D5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>02912624</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>http://owr.conservation.ca.gov/Well/WellDetailPage.aspx?domsapp=1&amp;apinum=02912624</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>2975558</v>
       </c>
@@ -507,11 +749,16 @@
       <c r="C6">
         <v>-118.87682</v>
       </c>
-      <c r="D6">
-        <v>2975558</v>
+      <c r="D6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>02975558</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>http://owr.conservation.ca.gov/Well/WellDetailPage.aspx?domsapp=1&amp;apinum=02975558</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>2914064</v>
       </c>
@@ -521,11 +768,16 @@
       <c r="C7">
         <v>-118.992262</v>
       </c>
-      <c r="D7">
-        <v>2914064</v>
+      <c r="D7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>02914064</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>http://owr.conservation.ca.gov/Well/WellDetailPage.aspx?domsapp=1&amp;apinum=02914064</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>3046608</v>
       </c>
@@ -535,11 +787,16 @@
       <c r="C8">
         <v>-118.813582</v>
       </c>
-      <c r="D8">
-        <v>3046608</v>
+      <c r="D8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>03046608</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>http://owr.conservation.ca.gov/Well/WellDetailPage.aspx?domsapp=1&amp;apinum=03046608</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>2966045</v>
       </c>
@@ -549,8 +806,13 @@
       <c r="C9">
         <v>-118.812211</v>
       </c>
-      <c r="D9">
-        <v>2966045</v>
+      <c r="D9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>02966045</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>http://owr.conservation.ca.gov/Well/WellDetailPage.aspx?domsapp=1&amp;apinum=02966045</v>
       </c>
     </row>
   </sheetData>

</xml_diff>